<commit_message>
Feat(v3) : Slave Step 파티션 나누기
</commit_message>
<xml_diff>
--- a/src/main/resources/UwayType.xlsx
+++ b/src/main/resources/UwayType.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jun\IdeaProjects\2022-University-entrance-exam-ratio-crawling-project\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jun\IdeaProjects\daehagnawa-batch\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16791E8-7B34-41B2-8AC0-41D36B39EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFA65F1-D63B-4FA9-883E-35F0EB608E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2880" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>